<commit_message>
Added The Screenshot Method to Selenium Functions
</commit_message>
<xml_diff>
--- a/test/mac_repair/selenium/TC02_test_cases.xlsx
+++ b/test/mac_repair/selenium/TC02_test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EEWorkspace\mac_repair\test\mac_repair\selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495B92D0-2333-401C-A649-1518B606715B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FD5AD4-F79C-4E56-906C-808B942C50CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2808" yWindow="2868" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
     <t>R</t>
   </si>
   <si>
-    <t>repTest</t>
+    <t>newrep</t>
   </si>
 </sst>
 </file>

</xml_diff>